<commit_message>
Se agrego el OVLO UVLO en el archivo LDOA_with_OVLO*
</commit_message>
<xml_diff>
--- a/Calculos para UVLO OVLO.xlsx
+++ b/Calculos para UVLO OVLO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agust\Documents\Facultad\Diseño de Circuitos Electronicos\Trabajo Práctico\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agust\Documents\Facultad\Diseño de Circuitos Electronicos\DISE-O_CIRCUITOS_ELECTRONICOS_1C_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03E47FCC-8EB4-45E8-A9F7-355E3CB0C0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CAE98E-9779-4103-AB4D-A05B83BA2633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9077941B-81D1-4A26-BF84-8A1B86E974CC}"/>
+    <workbookView xWindow="-5565" yWindow="1770" windowWidth="15375" windowHeight="7875" xr2:uid="{9077941B-81D1-4A26-BF84-8A1B86E974CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>RT</t>
   </si>
@@ -65,13 +65,37 @@
   </si>
   <si>
     <t>UVLO</t>
+  </si>
+  <si>
+    <t>VARIABLE</t>
+  </si>
+  <si>
+    <t>VALOR 5V</t>
+  </si>
+  <si>
+    <t>VALOR 3,3V</t>
+  </si>
+  <si>
+    <t>TIP.</t>
+  </si>
+  <si>
+    <t>MIN.</t>
+  </si>
+  <si>
+    <t>MAX.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>V_REG (V)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,16 +103,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -96,20 +155,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="60% - Énfasis2" xfId="2" builtinId="36"/>
+    <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -120,6 +233,43 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93A86ABD-66BE-4C91-8D5A-A3F8E83D7DF0}" name="Tabla1" displayName="Tabla1" ref="B1:D7" totalsRowShown="0">
+  <autoFilter ref="B1:D7" xr:uid="{93A86ABD-66BE-4C91-8D5A-A3F8E83D7DF0}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D401250C-02CD-4026-AA48-A4677D664BC2}" name="VARIABLE" dataDxfId="7" dataCellStyle="60% - Énfasis2"/>
+    <tableColumn id="2" xr3:uid="{D164A934-58AD-49A3-BF31-4314FC5FC84F}" name="VALOR 5V" dataDxfId="6" dataCellStyle="Cálculo"/>
+    <tableColumn id="3" xr3:uid="{BE8B943F-9D68-41AD-8DE0-2E194FC56D30}" name="VALOR 3,3V"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DFE87A79-2086-4EB9-B114-8333B3954BFF}" name="Tabla2" displayName="Tabla2" ref="B8:D14" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+  <autoFilter ref="B8:D14" xr:uid="{DFE87A79-2086-4EB9-B114-8333B3954BFF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{3CA15A23-C0C0-4E10-9EBA-2AC840ADE182}" name="VARIABLE" dataDxfId="5" dataCellStyle="60% - Énfasis2"/>
+    <tableColumn id="2" xr3:uid="{269EFACA-D594-4119-B9FF-250108C24FE8}" name="VALOR 5V" dataDxfId="4" dataCellStyle="Cálculo"/>
+    <tableColumn id="3" xr3:uid="{DE3E5F05-DE90-4C1C-B03A-C5C05D682648}" name="VALOR 3,3V" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DF443149-AF39-4BEC-805D-3AD168C6CB45}" name="Tabla4" displayName="Tabla4" ref="G1:J2" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="G1:J2" xr:uid="{DF443149-AF39-4BEC-805D-3AD168C6CB45}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C879B20E-68FF-48E2-9FE3-9A6DADB957AF}" name="VARIABLE"/>
+    <tableColumn id="2" xr3:uid="{B18F12C6-08FD-43FE-9514-266973F6FD5F}" name="MIN."/>
+    <tableColumn id="3" xr3:uid="{06A82989-8F76-4F15-92D4-64A897F02D32}" name="TIP."/>
+    <tableColumn id="4" xr3:uid="{CB0DFFF5-925B-4EC1-BA1D-9749C69B9E44}" name="MAX."/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,128 +569,220 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93A350C-A999-4639-A83D-2E9C14278F41}">
-  <dimension ref="A2:C14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>10000</v>
+      </c>
+      <c r="D5" s="6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <f>C5/((C3/C2)-1)</f>
+        <v>3243.2432432432424</v>
+      </c>
+      <c r="D6" s="6">
+        <f>D5/((D3/D2)-1)</f>
+        <v>5217.3913043478251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6">
+        <f>(C5/((C4/C2)-1))-C6</f>
+        <v>185.32818532818601</v>
+      </c>
+      <c r="D7" s="6">
+        <f>(D5/((D4/D2)-1))-D6</f>
+        <v>237.15415019762895</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" t="s">
+      <c r="D9" s="6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4.8</v>
+      </c>
+      <c r="D10" s="6">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="D11" s="6">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" t="s">
+      <c r="C12" s="6">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6">
-        <f>C5/((C3/C2)-1)</f>
-        <v>9615.3846153846152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" t="s">
+      <c r="C13" s="7">
+        <f>C12/((C11/C9)-1)</f>
+        <v>1136.3636363636363</v>
+      </c>
+      <c r="D13" s="6">
+        <f>D12/((D11/D9)-1)</f>
+        <v>4166.666666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7">
-        <f>(C5/((C4/C2)-1))-C6</f>
-        <v>801.282051282049</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <f>C12/((C11/C9)-1)</f>
-        <v>11363.636363636362</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <f>(C12*C13)/(((C10/C9)-1)*C13-C12)</f>
-        <v>250000.00000000125</v>
+        <v>25000.000000000098</v>
+      </c>
+      <c r="D14" s="6">
+        <f>(D12*D13)/(((D10/D9)-1)*D13-D12)</f>
+        <v>24999.999999999956</v>
       </c>
     </row>
   </sheetData>
@@ -549,5 +791,11 @@
     <mergeCell ref="A9:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cambios en el archivo de calculos para OVLO UVLO
</commit_message>
<xml_diff>
--- a/Calculos para UVLO OVLO.xlsx
+++ b/Calculos para UVLO OVLO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agust\Documents\Facultad\Diseño de Circuitos Electronicos\DISE-O_CIRCUITOS_ELECTRONICOS_1C_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CAE98E-9779-4103-AB4D-A05B83BA2633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4D44D6-41CF-4700-8F19-250C28AAA05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5565" yWindow="1770" windowWidth="15375" windowHeight="7875" xr2:uid="{9077941B-81D1-4A26-BF84-8A1B86E974CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9077941B-81D1-4A26-BF84-8A1B86E974CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>RT</t>
   </si>
@@ -89,6 +89,45 @@
   </si>
   <si>
     <t>V_REG (V)</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>SELA(V)</t>
+  </si>
+  <si>
+    <t>V_f(V)</t>
+  </si>
+  <si>
+    <t>V_O(V)</t>
+  </si>
+  <si>
+    <t>R_UP</t>
+  </si>
+  <si>
+    <t>R_DOWN</t>
+  </si>
+  <si>
+    <t>R_UP(ohm)</t>
+  </si>
+  <si>
+    <t>R_DOWN(ohm)</t>
+  </si>
+  <si>
+    <t>V_OUT</t>
+  </si>
+  <si>
+    <t>V_REF</t>
+  </si>
+  <si>
+    <t>V_Z</t>
+  </si>
+  <si>
+    <t>OVLO_DOWN</t>
+  </si>
+  <si>
+    <t>OVLO_UP</t>
   </si>
 </sst>
 </file>
@@ -185,19 +224,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% - Énfasis2" xfId="2" builtinId="36"/>
     <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -239,8 +288,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93A86ABD-66BE-4C91-8D5A-A3F8E83D7DF0}" name="Tabla1" displayName="Tabla1" ref="B1:D7" totalsRowShown="0">
   <autoFilter ref="B1:D7" xr:uid="{93A86ABD-66BE-4C91-8D5A-A3F8E83D7DF0}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D401250C-02CD-4026-AA48-A4677D664BC2}" name="VARIABLE" dataDxfId="7" dataCellStyle="60% - Énfasis2"/>
-    <tableColumn id="2" xr3:uid="{D164A934-58AD-49A3-BF31-4314FC5FC84F}" name="VALOR 5V" dataDxfId="6" dataCellStyle="Cálculo"/>
+    <tableColumn id="1" xr3:uid="{D401250C-02CD-4026-AA48-A4677D664BC2}" name="VARIABLE" dataDxfId="10" dataCellStyle="60% - Énfasis2"/>
+    <tableColumn id="2" xr3:uid="{D164A934-58AD-49A3-BF31-4314FC5FC84F}" name="VALOR 5V" dataDxfId="9" dataCellStyle="Cálculo"/>
     <tableColumn id="3" xr3:uid="{BE8B943F-9D68-41AD-8DE0-2E194FC56D30}" name="VALOR 3,3V"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -248,25 +297,37 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DFE87A79-2086-4EB9-B114-8333B3954BFF}" name="Tabla2" displayName="Tabla2" ref="B8:D14" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DFE87A79-2086-4EB9-B114-8333B3954BFF}" name="Tabla2" displayName="Tabla2" ref="B8:D14" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B8:D14" xr:uid="{DFE87A79-2086-4EB9-B114-8333B3954BFF}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3CA15A23-C0C0-4E10-9EBA-2AC840ADE182}" name="VARIABLE" dataDxfId="5" dataCellStyle="60% - Énfasis2"/>
-    <tableColumn id="2" xr3:uid="{269EFACA-D594-4119-B9FF-250108C24FE8}" name="VALOR 5V" dataDxfId="4" dataCellStyle="Cálculo"/>
-    <tableColumn id="3" xr3:uid="{DE3E5F05-DE90-4C1C-B03A-C5C05D682648}" name="VALOR 3,3V" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3CA15A23-C0C0-4E10-9EBA-2AC840ADE182}" name="VARIABLE" dataDxfId="6" dataCellStyle="60% - Énfasis2"/>
+    <tableColumn id="2" xr3:uid="{269EFACA-D594-4119-B9FF-250108C24FE8}" name="VALOR 5V" dataDxfId="5" dataCellStyle="Cálculo"/>
+    <tableColumn id="3" xr3:uid="{DE3E5F05-DE90-4C1C-B03A-C5C05D682648}" name="VALOR 3,3V" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DF443149-AF39-4BEC-805D-3AD168C6CB45}" name="Tabla4" displayName="Tabla4" ref="G1:J2" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DF443149-AF39-4BEC-805D-3AD168C6CB45}" name="Tabla4" displayName="Tabla4" ref="G1:J2" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="G1:J2" xr:uid="{DF443149-AF39-4BEC-805D-3AD168C6CB45}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C879B20E-68FF-48E2-9FE3-9A6DADB957AF}" name="VARIABLE"/>
     <tableColumn id="2" xr3:uid="{B18F12C6-08FD-43FE-9514-266973F6FD5F}" name="MIN."/>
     <tableColumn id="3" xr3:uid="{06A82989-8F76-4F15-92D4-64A897F02D32}" name="TIP."/>
     <tableColumn id="4" xr3:uid="{CB0DFFF5-925B-4EC1-BA1D-9749C69B9E44}" name="MAX."/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0D0FF11E-EF2E-45DC-A8AA-126DF7F8506F}" name="Tabla3" displayName="Tabla3" ref="B16:D21" totalsRowShown="0">
+  <autoFilter ref="B16:D21" xr:uid="{0D0FF11E-EF2E-45DC-A8AA-126DF7F8506F}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{CDE7B751-AA8E-4F5B-B21B-D9D004CFC85B}" name="Variable" dataDxfId="2" dataCellStyle="60% - Énfasis2"/>
+    <tableColumn id="2" xr3:uid="{EF2F3F68-78B8-4963-B8BD-7337639CA096}" name="VALOR 5V" dataDxfId="1" dataCellStyle="Cálculo"/>
+    <tableColumn id="3" xr3:uid="{37FCB375-0C40-46CA-889D-2A5F35BE0C86}" name="VALOR 3,3V" dataDxfId="0" dataCellStyle="Cálculo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -569,15 +630,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93A350C-A999-4639-A83D-2E9C14278F41}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
@@ -606,16 +669,16 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>1.2</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>1.2</v>
       </c>
       <c r="G2" t="s">
@@ -632,67 +695,67 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>3.5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>4.7</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>3.4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>10000</v>
       </c>
-      <c r="D5" s="6">
-        <v>10000</v>
+      <c r="D5" s="5">
+        <v>5900</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <f>C5/((C3/C2)-1)</f>
         <v>3243.2432432432424</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <f>D5/((D3/D2)-1)</f>
-        <v>5217.3913043478251</v>
+        <v>3078.260869565217</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <f>(C5/((C4/C2)-1))-C6</f>
         <v>185.32818532818601</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <f>(D5/((D4/D2)-1))-D6</f>
-        <v>237.15415019762895</v>
+        <v>139.92094861660098</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -708,81 +771,209 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>2.5</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>2.5</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>4.8</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>3.2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>4.7</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>3.1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>1000</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <f>C12/((C11/C9)-1)</f>
         <v>1136.3636363636363</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <f>D12/((D11/D9)-1)</f>
         <v>4166.666666666667</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <f>(C12*C13)/(((C10/C9)-1)*C13-C12)</f>
         <v>25000.000000000098</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <f>(D12*D13)/(((D10/D9)-1)*D13-D12)</f>
         <v>24999.999999999956</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="5">
+        <f>C17*C21/(C20+C21)</f>
+        <v>1.2023939064200218</v>
+      </c>
+      <c r="D18" s="5">
+        <f>D17*D21/(D20+D21)</f>
+        <v>1.2079019073569481</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="5">
+        <v>5</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="5">
+        <v>6980</v>
+      </c>
+      <c r="D20" s="5">
+        <v>6980</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="6">
+        <v>2210</v>
+      </c>
+      <c r="D21" s="5">
+        <f>2210+1820</f>
+        <v>4030</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23">
+        <v>2.5</v>
+      </c>
+      <c r="D23">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24">
+        <v>1.25</v>
+      </c>
+      <c r="D24">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>10000</v>
+      </c>
+      <c r="D25">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <f>C25*((C23/C24)-1)</f>
+        <v>10000</v>
+      </c>
+      <c r="D26">
+        <f>D25*((D23/D24)-1)</f>
+        <v>10491.803278688523</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -792,10 +983,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
imagenes de las partes del circuito
</commit_message>
<xml_diff>
--- a/Calculos para UVLO OVLO.xlsx
+++ b/Calculos para UVLO OVLO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agust\Documents\Facultad\Diseño de Circuitos Electronicos\DISE-O_CIRCUITOS_ELECTRONICOS_1C_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEAA05B-9FC8-435A-B012-00D6DA367066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8631F9A7-F103-4C4A-A238-A7E697343CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9077941B-81D1-4A26-BF84-8A1B86E974CC}"/>
+    <workbookView xWindow="2250" yWindow="-405" windowWidth="15375" windowHeight="7875" xr2:uid="{9077941B-81D1-4A26-BF84-8A1B86E974CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93A350C-A999-4639-A83D-2E9C14278F41}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36:H42"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1145,7 @@
         <v>40</v>
       </c>
       <c r="J32">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="J34">
         <f>(J31-J32)/J30  - J33</f>
-        <v>26.262189215369716</v>
+        <v>27.271230222796255</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>